<commit_message>
small bugfix and changes for q2
</commit_message>
<xml_diff>
--- a/Q2/images/calculations.xlsx
+++ b/Q2/images/calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zceetlc\Documents\GitHub\COMP0037_CW1\Q2\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F667E086-526D-48EC-9F30-C34D7BE0BB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BD08E6-FB50-4E55-8200-4AD1D57D0127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19140" yWindow="5460" windowWidth="21600" windowHeight="11490" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26490" yWindow="5430" windowWidth="21600" windowHeight="11490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells Visited" sheetId="1" r:id="rId1"/>
@@ -402,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1159,7 +1159,7 @@
         <v>1558</v>
       </c>
       <c r="J27" s="1">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K27" s="1">
         <v>47</v>
@@ -1224,7 +1224,7 @@
       </c>
       <c r="J29" s="1">
         <f t="shared" ref="J29:K29" si="1">SUM(J3:J28)</f>
-        <v>12147</v>
+        <v>12146</v>
       </c>
       <c r="K29" s="1">
         <f t="shared" si="1"/>
@@ -1240,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EAB3DF9-0800-49AE-A0B6-0B07B55B1D91}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>